<commit_message>
Added Singapore trip's Ritual
</commit_message>
<xml_diff>
--- a/Time Table May 2018.xlsx
+++ b/Time Table May 2018.xlsx
@@ -5471,8 +5471,8 @@
       <xdr:rowOff>7620</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>22860</xdr:colOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>609600</xdr:colOff>
       <xdr:row>33</xdr:row>
       <xdr:rowOff>426720</xdr:rowOff>
     </xdr:to>
@@ -5483,12 +5483,17 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="693420" y="1333500"/>
-          <a:ext cx="3307080" cy="419100"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
+          <a:off x="694509" y="14735991"/>
+          <a:ext cx="2571205" cy="419100"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent4">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
       </xdr:spPr>
       <xdr:style>
         <a:lnRef idx="2">
@@ -6192,14 +6197,14 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>327660</xdr:colOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>305889</xdr:colOff>
       <xdr:row>32</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>342900</xdr:colOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>321129</xdr:colOff>
       <xdr:row>32</xdr:row>
       <xdr:rowOff>419100</xdr:rowOff>
     </xdr:to>
@@ -6210,8 +6215,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="13586460" y="883920"/>
-          <a:ext cx="678180" cy="419100"/>
+          <a:off x="12258403" y="14282057"/>
+          <a:ext cx="679269" cy="419100"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -6311,16 +6316,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>15240</xdr:colOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>37011</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>414745</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>13063</xdr:colOff>
       <xdr:row>32</xdr:row>
-      <xdr:rowOff>22860</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>655320</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>391885</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -6329,8 +6334,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="12611100" y="906780"/>
-          <a:ext cx="640080" cy="419100"/>
+          <a:off x="11325497" y="14250488"/>
+          <a:ext cx="640080" cy="423454"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -6963,73 +6968,73 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>378822</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>443048</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>111033</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>415834</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="688" name="สี่เหลี่ยมผืนผ้า 687"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11003279" y="14278791"/>
+          <a:ext cx="396240" cy="419100"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="th-TH" sz="1000"/>
+            <a:t>กินข้าวแ</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>648789</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>412569</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
       <xdr:col>18</xdr:col>
-      <xdr:colOff>259080</xdr:colOff>
+      <xdr:colOff>412569</xdr:colOff>
       <xdr:row>32</xdr:row>
-      <xdr:rowOff>7620</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>655320</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>426720</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="688" name="สี่เหลี่ยมผืนผ้า 687"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="12192000" y="891540"/>
-          <a:ext cx="396240" cy="419100"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:r>
-            <a:rPr lang="th-TH" sz="1000"/>
-            <a:t>กินข้าวแ</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>594360</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>434340</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>358140</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>411480</xdr:rowOff>
+      <xdr:rowOff>389709</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -7038,8 +7043,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="13190220" y="876300"/>
-          <a:ext cx="426720" cy="419100"/>
+          <a:off x="11937275" y="14248312"/>
+          <a:ext cx="427808" cy="423454"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -10848,14 +10853,14 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>381000</xdr:colOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>228599</xdr:colOff>
       <xdr:row>25</xdr:row>
       <xdr:rowOff>22860</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>358140</xdr:colOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>205740</xdr:colOff>
       <xdr:row>26</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
@@ -10866,8 +10871,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="13639800" y="15491460"/>
-          <a:ext cx="640080" cy="419100"/>
+          <a:off x="12845142" y="11180717"/>
+          <a:ext cx="641169" cy="423454"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -11304,16 +11309,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>185058</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>435428</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
       <xdr:col>22</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:colOff>161109</xdr:colOff>
       <xdr:row>25</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>22</xdr:col>
-      <xdr:colOff>640080</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>419100</xdr:rowOff>
+      <xdr:rowOff>408214</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -11322,7 +11327,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="14584680" y="15468600"/>
+          <a:off x="14129658" y="11146971"/>
           <a:ext cx="640080" cy="419100"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -11532,16 +11537,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>22</xdr:col>
-      <xdr:colOff>381000</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>434340</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
       <xdr:col>23</xdr:col>
-      <xdr:colOff>655320</xdr:colOff>
+      <xdr:colOff>446315</xdr:colOff>
       <xdr:row>28</xdr:row>
-      <xdr:rowOff>411480</xdr:rowOff>
+      <xdr:rowOff>20683</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>56606</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>444137</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -11550,8 +11555,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="14965680" y="16786860"/>
-          <a:ext cx="937260" cy="419100"/>
+          <a:off x="15718972" y="12517483"/>
+          <a:ext cx="938348" cy="423454"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -11931,16 +11936,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>354875</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>10886</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
       <xdr:col>21</xdr:col>
-      <xdr:colOff>289560</xdr:colOff>
+      <xdr:colOff>118655</xdr:colOff>
       <xdr:row>25</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>22</xdr:col>
-      <xdr:colOff>53340</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>419100</xdr:rowOff>
+      <xdr:rowOff>429986</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -11949,8 +11954,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="14211300" y="15468600"/>
-          <a:ext cx="426720" cy="419100"/>
+          <a:off x="13635446" y="11168743"/>
+          <a:ext cx="427809" cy="419100"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -13146,63 +13151,6 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>381000</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>22860</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>358140</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="827" name="สี่เหลี่ยมผืนผ้า 826"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="13639800" y="15491460"/>
-          <a:ext cx="640080" cy="419100"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:r>
-            <a:rPr lang="th-TH" sz="1000"/>
-            <a:t>เดินทาง</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
       <xdr:col>19</xdr:col>
       <xdr:colOff>15240</xdr:colOff>
       <xdr:row>12</xdr:row>
@@ -13603,13 +13551,13 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>22</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:colOff>239486</xdr:colOff>
       <xdr:row>15</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>22</xdr:col>
-      <xdr:colOff>640080</xdr:colOff>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>215538</xdr:colOff>
       <xdr:row>15</xdr:row>
       <xdr:rowOff>419100</xdr:rowOff>
     </xdr:to>
@@ -13620,7 +13568,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="14584680" y="15468600"/>
+          <a:off x="14848115" y="6694714"/>
           <a:ext cx="640080" cy="419100"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -14230,15 +14178,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>21</xdr:col>
-      <xdr:colOff>289560</xdr:colOff>
+      <xdr:colOff>474617</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>402772</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>238397</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>22</xdr:col>
-      <xdr:colOff>53340</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>419100</xdr:rowOff>
+      <xdr:rowOff>375558</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -14247,8 +14195,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="14211300" y="15468600"/>
-          <a:ext cx="426720" cy="419100"/>
+          <a:off x="14419217" y="6651172"/>
+          <a:ext cx="427809" cy="419100"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14678,6 +14626,11 @@
             <a:rPr lang="th-TH" sz="800"/>
             <a:t>หากนอนที่สนามบิน มันเร็วก็จริง แต่เสียอย่างคือ มื้อเช้าจะแพง อยู่ที่สถานการณ์การเงิน โอเคมั้ย</a:t>
           </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="800"/>
+            <a:t> https://travel.kapook.com/view104611.html </a:t>
+          </a:r>
+          <a:endParaRPr lang="th-TH" sz="800"/>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -14686,13 +14639,13 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>601980</xdr:colOff>
+      <xdr:colOff>468087</xdr:colOff>
       <xdr:row>33</xdr:row>
       <xdr:rowOff>7620</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>533400</xdr:colOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>10888</xdr:colOff>
       <xdr:row>33</xdr:row>
       <xdr:rowOff>426720</xdr:rowOff>
     </xdr:to>
@@ -14703,8 +14656,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5905500" y="14592300"/>
-          <a:ext cx="1257300" cy="419100"/>
+          <a:off x="5780316" y="14735991"/>
+          <a:ext cx="1534886" cy="419100"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14742,7 +14695,7 @@
           </a:r>
           <a:r>
             <a:rPr lang="en-US" sz="1000" baseline="0"/>
-            <a:t> in in DMK Airport</a:t>
+            <a:t> in in DMK Airport  (Passport + E-Ticket) </a:t>
           </a:r>
           <a:endParaRPr lang="th-TH" sz="1000"/>
         </a:p>
@@ -14998,11 +14951,26 @@
           <a:pPr algn="l"/>
           <a:r>
             <a:rPr lang="th-TH" sz="1000"/>
-            <a:t>แลกเงิน </a:t>
+            <a:t>แลกเงิน</a:t>
           </a:r>
           <a:r>
             <a:rPr lang="en-US" sz="1000"/>
-            <a:t>SGD 4800</a:t>
+            <a:t> 210</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="th-TH" sz="1000"/>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1000"/>
+            <a:t>SGD </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1000"/>
+            <a:t>5100</a:t>
           </a:r>
           <a:r>
             <a:rPr lang="en-US" sz="1000" baseline="0"/>
@@ -15085,7 +15053,7 @@
           </a:r>
           <a:r>
             <a:rPr lang="en-US" sz="1000"/>
-            <a:t>4800</a:t>
+            <a:t>5100</a:t>
           </a:r>
           <a:r>
             <a:rPr lang="en-US" sz="1000" baseline="0"/>
@@ -15427,14 +15395,14 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>647700</xdr:colOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>157843</xdr:colOff>
       <xdr:row>16</xdr:row>
       <xdr:rowOff>15240</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>624840</xdr:colOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>134983</xdr:colOff>
       <xdr:row>16</xdr:row>
       <xdr:rowOff>434340</xdr:rowOff>
     </xdr:to>
@@ -15445,8 +15413,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5288280" y="7086600"/>
-          <a:ext cx="640080" cy="419100"/>
+          <a:off x="7462157" y="7156269"/>
+          <a:ext cx="641169" cy="419100"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -16123,16 +16091,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>281940</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>426720</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>274320</xdr:colOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>76201</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>403860</xdr:rowOff>
+      <xdr:rowOff>185056</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>391886</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>44630</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -16141,8 +16109,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="10226040" y="6614160"/>
-          <a:ext cx="1318260" cy="419100"/>
+          <a:off x="6052458" y="6879770"/>
+          <a:ext cx="2307771" cy="305889"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -16178,7 +16146,11 @@
           </a:r>
           <a:r>
             <a:rPr lang="en-US" sz="1000" baseline="0"/>
-            <a:t> 1111</a:t>
+            <a:t> 1111 </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="th-TH" sz="1000" baseline="0"/>
+            <a:t>(แคค่ทางโทรศัพท์ก็พอ)</a:t>
           </a:r>
           <a:endParaRPr lang="th-TH" sz="1000"/>
         </a:p>
@@ -16457,16 +16429,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>251460</xdr:colOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>567146</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>30480</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>277860</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>434040</xdr:rowOff>
+      <xdr:rowOff>422365</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>593546</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>379611</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -16475,8 +16447,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7543800" y="5775960"/>
-          <a:ext cx="2015220" cy="403560"/>
+          <a:off x="9199517" y="6224451"/>
+          <a:ext cx="2018486" cy="403560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -16864,14 +16836,14 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>441960</xdr:colOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>137160</xdr:colOff>
       <xdr:row>32</xdr:row>
       <xdr:rowOff>15240</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>563880</xdr:colOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>259080</xdr:colOff>
       <xdr:row>32</xdr:row>
       <xdr:rowOff>396240</xdr:rowOff>
     </xdr:to>
@@ -16882,8 +16854,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5745480" y="14157960"/>
-          <a:ext cx="1447800" cy="381000"/>
+          <a:off x="6113417" y="14297297"/>
+          <a:ext cx="1449977" cy="381000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -16932,16 +16904,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>624840</xdr:colOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>505097</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>57694</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>352698</xdr:colOff>
       <xdr:row>32</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>472440</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>419100</xdr:rowOff>
+      <xdr:rowOff>38100</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -16950,8 +16922,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9906000" y="14142720"/>
-          <a:ext cx="1836420" cy="419100"/>
+          <a:off x="7145383" y="13893437"/>
+          <a:ext cx="1839686" cy="426720"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -17075,16 +17047,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>22</xdr:col>
-      <xdr:colOff>190500</xdr:colOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>332016</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>165463</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>642258</xdr:colOff>
       <xdr:row>31</xdr:row>
-      <xdr:rowOff>426720</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>23</xdr:col>
-      <xdr:colOff>472440</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>403860</xdr:rowOff>
+      <xdr:rowOff>142603</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -17093,8 +17065,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="14775180" y="14127480"/>
-          <a:ext cx="944880" cy="419100"/>
+          <a:off x="8964387" y="13554892"/>
+          <a:ext cx="2302328" cy="423454"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -17128,6 +17100,14 @@
           <a:pPr algn="l"/>
           <a:r>
             <a:rPr lang="th-TH" sz="1000"/>
+            <a:t>ได้ </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1000"/>
+            <a:t>... </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="th-TH" sz="1000"/>
             <a:t>เดินทาง</a:t>
           </a:r>
           <a:r>
@@ -17137,6 +17117,22 @@
           <a:r>
             <a:rPr lang="th-TH" sz="1000"/>
             <a:t>กระเป๋า</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1000"/>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="th-TH" sz="1000"/>
+            <a:t>ถึง </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1000"/>
+            <a:t>22 </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="th-TH" sz="1000"/>
+            <a:t>โมง (ต้องคำนึงเรื่องความปลอดภภภัยมากๆ)</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -18878,16 +18874,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>106680</xdr:colOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>357051</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>45720</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>228600</xdr:colOff>
+      <xdr:rowOff>56606</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>478971</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>426720</xdr:rowOff>
+      <xdr:rowOff>437606</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -18896,8 +18892,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6073140" y="5791200"/>
-          <a:ext cx="1447800" cy="381000"/>
+          <a:off x="8325394" y="5858692"/>
+          <a:ext cx="1449977" cy="381000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -18947,15 +18943,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>99060</xdr:colOff>
+      <xdr:colOff>490948</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>316774</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>272145</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>22860</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>220980</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>403860</xdr:rowOff>
+      <xdr:rowOff>251460</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -18964,8 +18960,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6065520" y="6652260"/>
-          <a:ext cx="1447800" cy="381000"/>
+          <a:off x="6467205" y="6565174"/>
+          <a:ext cx="1109254" cy="381000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -19080,27 +19076,84 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>138250</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>432163</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>114301</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>404949</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="311" name="สี่เหลี่ยมผืนผ้า 310"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7442564" y="6234249"/>
+          <a:ext cx="640080" cy="419100"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="th-TH" sz="1000"/>
+            <a:t>เดินทาง</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>106680</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>11</xdr:col>
+      <xdr:col>10</xdr:col>
       <xdr:colOff>228600</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>381000</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="310" name="CustomShape 1"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="6073140" y="6187440"/>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>7620</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>350520</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>388620</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="313" name="CustomShape 1"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6858000" y="9730740"/>
           <a:ext cx="1447800" cy="381000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -19132,7 +19185,908 @@
               </a:solidFill>
               <a:latin typeface="Calibri"/>
             </a:rPr>
-            <a:t>relax do</a:t>
+            <a:t>relax</a:t>
+          </a:r>
+          <a:endParaRPr/>
+        </a:p>
+        <a:p>
+          <a:pPr>
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+          </a:pPr>
+          <a:endParaRPr/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>434340</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>15240</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>563880</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>418800</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="314" name="CustomShape 1"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11041380" y="7970520"/>
+          <a:ext cx="1455420" cy="403560"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="E46C0A"/>
+        </a:solidFill>
+        <a:ln w="25560">
+          <a:solidFill>
+            <a:srgbClr val="3A5F8B"/>
+          </a:solidFill>
+          <a:round/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr lIns="90000" tIns="45000" rIns="90000" bIns="45000"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="th-TH" sz="1100">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+            </a:rPr>
+            <a:t>ติว </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+            </a:rPr>
+            <a:t>HCI</a:t>
+          </a:r>
+          <a:endParaRPr/>
+        </a:p>
+        <a:p>
+          <a:pPr>
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+          </a:pPr>
+          <a:endParaRPr/>
+        </a:p>
+        <a:p>
+          <a:pPr>
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+          </a:pPr>
+          <a:endParaRPr/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>56607</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>425631</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>33746</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>402771</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="315" name="สี่เหลี่ยมผืนผ้า 314"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7360921" y="7566660"/>
+          <a:ext cx="641168" cy="423454"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="th-TH" sz="1000"/>
+            <a:t>เดินทาง</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>638992</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>10886</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>616132</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>429986</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="316" name="สี่เหลี่ยมผืนผ้า 315"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7279278" y="8044543"/>
+          <a:ext cx="641168" cy="419100"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="th-TH" sz="1000"/>
+            <a:t>เดินทาง</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>220980</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>30480</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>411480</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="317" name="CustomShape 1"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6187440" y="11521440"/>
+          <a:ext cx="1447800" cy="381000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="00B050"/>
+        </a:solidFill>
+        <a:ln w="25560">
+          <a:solidFill>
+            <a:srgbClr val="3A5F8B"/>
+          </a:solidFill>
+          <a:round/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr lIns="90000" tIns="45000" rIns="90000" bIns="45000"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+            </a:rPr>
+            <a:t>relax</a:t>
+          </a:r>
+          <a:endParaRPr/>
+        </a:p>
+        <a:p>
+          <a:pPr>
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+          </a:pPr>
+          <a:endParaRPr/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>533400</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>53340</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>419100</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="318" name="สี่เหลี่ยมผืนผ้า 317"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7825740" y="11490960"/>
+          <a:ext cx="2834640" cy="419100"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1000"/>
+            <a:t>Pack </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="th-TH" sz="1000"/>
+            <a:t>ของ และคอม ใส่กระเป๋า</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="th-TH" sz="1000" baseline="0"/>
+            <a:t> (ห้ามใช้กระเป๋าเดินทาง)</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1000" baseline="0"/>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="th-TH" sz="1000" baseline="0"/>
+            <a:t>มีบอกที่ขีดเส้นใต้ใน </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1000" baseline="0"/>
+            <a:t>to do list</a:t>
+          </a:r>
+          <a:endParaRPr lang="th-TH" sz="1000"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>579119</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>413659</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>37012</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>348344</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="319" name="CustomShape 1"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="15187748" y="10232573"/>
+          <a:ext cx="1449978" cy="381000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="00B050"/>
+        </a:solidFill>
+        <a:ln w="25560">
+          <a:solidFill>
+            <a:srgbClr val="3A5F8B"/>
+          </a:solidFill>
+          <a:round/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr lIns="90000" tIns="45000" rIns="90000" bIns="45000"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+            </a:rPr>
+            <a:t>relax</a:t>
+          </a:r>
+          <a:endParaRPr/>
+        </a:p>
+        <a:p>
+          <a:pPr>
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+          </a:pPr>
+          <a:endParaRPr/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>89263</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>11974</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>357052</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>419889</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="320" name="CustomShape 1"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11377749" y="11169831"/>
+          <a:ext cx="931817" cy="407915"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="E46C0A"/>
+        </a:solidFill>
+        <a:ln w="25560">
+          <a:solidFill>
+            <a:srgbClr val="3A5F8B"/>
+          </a:solidFill>
+          <a:round/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr lIns="90000" tIns="45000" rIns="90000" bIns="45000"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="th-TH" sz="1100">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+            </a:rPr>
+            <a:t>ตามที่สหกิจที่มี</a:t>
+          </a:r>
+          <a:endParaRPr/>
+        </a:p>
+        <a:p>
+          <a:pPr>
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+          </a:pPr>
+          <a:endParaRPr/>
+        </a:p>
+        <a:p>
+          <a:pPr>
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+          </a:pPr>
+          <a:endParaRPr/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>357051</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>30481</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>556260</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>434041</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="321" name="CustomShape 1"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10317480" y="9849395"/>
+          <a:ext cx="863237" cy="403560"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="E46C0A"/>
+        </a:solidFill>
+        <a:ln w="25560">
+          <a:solidFill>
+            <a:srgbClr val="3A5F8B"/>
+          </a:solidFill>
+          <a:round/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr lIns="90000" tIns="45000" rIns="90000" bIns="45000"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="th-TH" sz="1100">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+            </a:rPr>
+            <a:t>ตามที่สหกิจที่มี</a:t>
+          </a:r>
+          <a:endParaRPr/>
+        </a:p>
+        <a:p>
+          <a:pPr>
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+          </a:pPr>
+          <a:endParaRPr/>
+        </a:p>
+        <a:p>
+          <a:pPr>
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+          </a:pPr>
+          <a:endParaRPr/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>3265</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>436518</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>644434</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>413658</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="322" name="สี่เหลี่ยมผืนผ้า 321"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="15939951" y="10701747"/>
+          <a:ext cx="641169" cy="423454"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="th-TH" sz="1000"/>
+            <a:t>ตัดเล็บ</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>411480</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>434340</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>388620</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>411480</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="323" name="สี่เหลี่ยมผืนผ้า 322"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="15659100" y="20322540"/>
+          <a:ext cx="640080" cy="419100"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="th-TH" sz="1000"/>
+            <a:t>ตัดเล็บ</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>547552</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>419100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>478972</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>396240</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="324" name="สี่เหลี่ยมผืนผ้า 323"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="15156181" y="5774871"/>
+          <a:ext cx="1259477" cy="423455"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="th-TH" sz="1000"/>
+            <a:t>สร้าง </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1000"/>
+            <a:t>Ritual </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="th-TH" sz="1000"/>
+            <a:t>สำหรับ ตอนอยู่สิงค์โปร์</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>559525</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>9797</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>490945</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>433251</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="325" name="สี่เหลี่ยมผืนผ้า 324"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="15168154" y="6258197"/>
+          <a:ext cx="1259477" cy="423454"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="th-TH" sz="1000"/>
+            <a:t>สร้าง </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1000"/>
+            <a:t>Ritual </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="th-TH" sz="1000"/>
+            <a:t>สำหรับ ตอนสหกิจ</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="th-TH" sz="1000" baseline="0"/>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1000" baseline="0"/>
+            <a:t>Part 1</a:t>
+          </a:r>
+          <a:endParaRPr lang="th-TH" sz="1000"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>544286</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>35922</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>391886</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>787</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="327" name="CustomShape 1"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7848600" y="5391693"/>
+          <a:ext cx="1175657" cy="411180"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="E46C0A"/>
+        </a:solidFill>
+        <a:ln w="25560">
+          <a:solidFill>
+            <a:srgbClr val="3A5F8B"/>
+          </a:solidFill>
+          <a:round/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr lIns="90000" tIns="45000" rIns="90000" bIns="45000"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="th-TH" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+            </a:rPr>
+            <a:t>ทำ </a:t>
           </a:r>
           <a:r>
             <a:rPr lang="en-US" sz="1100" baseline="0">
@@ -19141,7 +20095,7 @@
               </a:solidFill>
               <a:latin typeface="Calibri"/>
             </a:rPr>
-            <a:t> the kirby 64</a:t>
+            <a:t>front-end</a:t>
           </a:r>
           <a:endParaRPr/>
         </a:p>
@@ -19153,62 +20107,13 @@
           </a:pPr>
           <a:endParaRPr/>
         </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>7620</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>7620</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>647700</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>426720</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="311" name="สี่เหลี่ยมผืนผ้า 310"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="5311140" y="6195060"/>
-          <a:ext cx="640080" cy="419100"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:r>
-            <a:rPr lang="th-TH" sz="1000"/>
-            <a:t>เดินทาง</a:t>
-          </a:r>
+        <a:p>
+          <a:pPr>
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+          </a:pPr>
+          <a:endParaRPr/>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -19216,25 +20121,146 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>326572</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>21771</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>315686</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>425331</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="328" name="CustomShape 1"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8958943" y="10287000"/>
+          <a:ext cx="1981200" cy="403560"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="E46C0A"/>
+        </a:solidFill>
+        <a:ln w="25560">
+          <a:solidFill>
+            <a:srgbClr val="3A5F8B"/>
+          </a:solidFill>
+          <a:round/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr lIns="90000" tIns="45000" rIns="90000" bIns="45000"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="th-TH" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+            </a:rPr>
+            <a:t>ประสานงาน </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+            </a:rPr>
+            <a:t>Web App </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="th-TH" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+            </a:rPr>
+            <a:t>กับปราง</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+            </a:rPr>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="th-TH" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+            </a:rPr>
+            <a:t>เรื่อง </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+            </a:rPr>
+            <a:t>Controller</a:t>
+          </a:r>
+          <a:endParaRPr/>
+        </a:p>
+        <a:p>
+          <a:pPr>
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+          </a:pPr>
+          <a:endParaRPr/>
+        </a:p>
+        <a:p>
+          <a:pPr>
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+          </a:pPr>
+          <a:endParaRPr/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>205740</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>434340</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>14760</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>395820</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="312" name="CustomShape 1"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="4846320" y="6179820"/>
+      <xdr:colOff>179614</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>6531</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>651574</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>409971</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="329" name="CustomShape 1"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4827814" y="10271760"/>
           <a:ext cx="471960" cy="403440"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -19274,28 +20300,169 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>56605</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>3265</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>33746</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>422365</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="326" name="สี่เหลี่ยมผืนผ้า 325"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11345091" y="10268494"/>
+          <a:ext cx="1969226" cy="419100"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent2"/>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="th-TH" sz="1000"/>
+            <a:t>เตรียม </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1000"/>
+            <a:t>Hackaton Web App</a:t>
+          </a:r>
+          <a:endParaRPr lang="th-TH" sz="1000"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>228600</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>7620</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>350520</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>388620</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="313" name="CustomShape 1"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="6858000" y="9730740"/>
-          <a:ext cx="1447800" cy="381000"/>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>609600</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>43542</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>609599</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>788</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="330" name="CustomShape 1"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6585857" y="5845628"/>
+          <a:ext cx="1328056" cy="403560"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="E46C0A"/>
+        </a:solidFill>
+        <a:ln w="25560">
+          <a:solidFill>
+            <a:srgbClr val="3A5F8B"/>
+          </a:solidFill>
+          <a:round/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr lIns="90000" tIns="45000" rIns="90000" bIns="45000"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="th-TH" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+            </a:rPr>
+            <a:t>ทำใบนัดอันใหม่ที่ คลินิกเสนานิเวช</a:t>
+          </a:r>
+          <a:endParaRPr/>
+        </a:p>
+        <a:p>
+          <a:pPr>
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+          </a:pPr>
+          <a:endParaRPr/>
+        </a:p>
+        <a:p>
+          <a:pPr>
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+          </a:pPr>
+          <a:endParaRPr/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>379912</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>54429</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>501832</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>435429</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="331" name="CustomShape 1"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7684226" y="5410200"/>
+          <a:ext cx="1449977" cy="381000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -19344,26 +20511,26 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>434340</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>15240</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>563880</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>418800</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="314" name="CustomShape 1"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="11041380" y="7970520"/>
-          <a:ext cx="1455420" cy="403560"/>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>119742</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>438693</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>631370</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>403558</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="332" name="CustomShape 1"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="14064342" y="5794464"/>
+          <a:ext cx="1175657" cy="411180"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -19388,22 +20555,22 @@
             </a:lnSpc>
           </a:pPr>
           <a:r>
-            <a:rPr lang="th-TH" sz="1100">
+            <a:rPr lang="th-TH" sz="1100" baseline="0">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
               <a:latin typeface="Calibri"/>
             </a:rPr>
-            <a:t>ติว </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100">
+            <a:t>ทำ </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
               <a:latin typeface="Calibri"/>
             </a:rPr>
-            <a:t>HCI</a:t>
+            <a:t>front-end</a:t>
           </a:r>
           <a:endParaRPr/>
         </a:p>
@@ -19427,142 +20594,28 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>45720</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>22860</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>22860</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="315" name="สี่เหลี่ยมผืนผ้า 314"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="5349240" y="7536180"/>
-          <a:ext cx="640080" cy="419100"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:r>
-            <a:rPr lang="th-TH" sz="1000"/>
-            <a:t>เดินทาง</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>83820</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>60960</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>419100</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="316" name="สี่เหลี่ยมผืนผ้า 315"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="5387340" y="7955280"/>
-          <a:ext cx="640080" cy="419100"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:r>
-            <a:rPr lang="th-TH" sz="1000"/>
-            <a:t>เดินทาง</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>220980</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>30480</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>342900</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>411480</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="317" name="CustomShape 1"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="6187440" y="11521440"/>
-          <a:ext cx="1447800" cy="381000"/>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>466997</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>32657</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>588917</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>413657</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="333" name="CustomShape 1"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11091454" y="6281057"/>
+          <a:ext cx="1449977" cy="381000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -19611,26 +20664,189 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>533400</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>263434</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>427808</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>240574</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>400594</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="334" name="สี่เหลี่ยมผืนผ้า 333"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="14208034" y="9800408"/>
+          <a:ext cx="1969226" cy="419100"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent2"/>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="th-TH" sz="1000"/>
+            <a:t>รีบนอน</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>383177</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>166552</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>53340</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>419100</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="318" name="สี่เหลี่ยมผืนผ้า 317"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="7825740" y="11490960"/>
-          <a:ext cx="2834640" cy="419100"/>
+      <xdr:colOff>360317</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>139338</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="335" name="สี่เหลี่ยมผืนผ้า 334"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9015548" y="14002295"/>
+          <a:ext cx="1969226" cy="419100"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent4">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="th-TH" sz="1000"/>
+            <a:t>ไม่ดีกว่า</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1000"/>
+            <a:t>...</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1000" baseline="0"/>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="th-TH" sz="1000"/>
+            <a:t>รีบนอน</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1000"/>
+            <a:t> 18</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1000" baseline="0"/>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="th-TH" sz="1000" baseline="0"/>
+            <a:t>โมง ตื่น ตี </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1000" baseline="0"/>
+            <a:t>4-5 </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="th-TH" sz="1000" baseline="0"/>
+            <a:t>ออก </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1000" baseline="0"/>
+            <a:t>6-7 </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="th-TH" sz="1000" baseline="0"/>
+            <a:t>โมง</a:t>
+          </a:r>
+          <a:endParaRPr lang="th-TH" sz="1000"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>547552</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>5443</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>478972</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>428898</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="336" name="สี่เหลี่ยมผืนผ้า 335"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8515895" y="6700157"/>
+          <a:ext cx="1259477" cy="423455"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -19663,28 +20879,12 @@
         <a:p>
           <a:pPr algn="l"/>
           <a:r>
+            <a:rPr lang="th-TH" sz="1000"/>
+            <a:t>กฏในการนำของเข้าสนามบิน</a:t>
+          </a:r>
+          <a:r>
             <a:rPr lang="en-US" sz="1000"/>
-            <a:t>Pack </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="th-TH" sz="1000"/>
-            <a:t>ของ และคอม ใส่กระเป๋า</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="th-TH" sz="1000" baseline="0"/>
-            <a:t> (ห้ามใช้กระเป๋าเดินทาง)</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1000" baseline="0"/>
-            <a:t> </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="th-TH" sz="1000" baseline="0"/>
-            <a:t>มีบอกที่ขีดเส้นใต้ใน </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1000" baseline="0"/>
-            <a:t>to do list</a:t>
+            <a:t>??</a:t>
           </a:r>
           <a:endParaRPr lang="th-TH" sz="1000"/>
         </a:p>
@@ -19694,94 +20894,26 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>22</xdr:col>
-      <xdr:colOff>579119</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>413659</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>25</xdr:col>
-      <xdr:colOff>37012</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>348344</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="319" name="CustomShape 1"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="15187748" y="10232573"/>
-          <a:ext cx="1449978" cy="381000"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:srgbClr val="00B050"/>
-        </a:solidFill>
-        <a:ln w="25560">
-          <a:solidFill>
-            <a:srgbClr val="3A5F8B"/>
-          </a:solidFill>
-          <a:round/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:txBody>
-        <a:bodyPr lIns="90000" tIns="45000" rIns="90000" bIns="45000"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:lnSpc>
-              <a:spcPct val="100000"/>
-            </a:lnSpc>
-          </a:pPr>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-              <a:latin typeface="Calibri"/>
-            </a:rPr>
-            <a:t>relax</a:t>
-          </a:r>
-          <a:endParaRPr/>
-        </a:p>
-        <a:p>
-          <a:pPr>
-            <a:lnSpc>
-              <a:spcPct val="100000"/>
-            </a:lnSpc>
-          </a:pPr>
-          <a:endParaRPr/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>437606</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>55516</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>41366</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>17117</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="320" name="CustomShape 1"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="10398035" y="10320745"/>
-          <a:ext cx="931817" cy="407915"/>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>174170</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>427806</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>21770</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>392672</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="338" name="CustomShape 1"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5486399" y="6229892"/>
+          <a:ext cx="1175657" cy="411180"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -19806,13 +20938,22 @@
             </a:lnSpc>
           </a:pPr>
           <a:r>
-            <a:rPr lang="th-TH" sz="1100">
+            <a:rPr lang="th-TH" sz="1100" baseline="0">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
               <a:latin typeface="Calibri"/>
             </a:rPr>
-            <a:t>ตามที่สหกิจที่มี</a:t>
+            <a:t>ทำ </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+            </a:rPr>
+            <a:t>front-end</a:t>
           </a:r>
           <a:endParaRPr/>
         </a:p>
@@ -19836,28 +20977,95 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>603068</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>443049</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>261257</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>415834</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="339" name="สี่เหลี่ยมผืนผ้า 338"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="14547668" y="7137763"/>
+          <a:ext cx="2314303" cy="419100"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent4">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="th-TH" sz="1000"/>
+            <a:t>เตรียมเสื้อผ้าที่เหมาะสมที่สุดสำหรับทริป</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="th-TH" sz="1000" baseline="0"/>
+            <a:t> เก็ยไว้สำหรับวันนั้น เผื่อเวลา</a:t>
+          </a:r>
+          <a:endParaRPr lang="th-TH" sz="1000"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>357051</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>30481</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>556260</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>434041</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="321" name="CustomShape 1"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="10317480" y="9849395"/>
-          <a:ext cx="863237" cy="403560"/>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>163284</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>14148</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>10884</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>425328</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="340" name="CustomShape 1"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5475513" y="7155177"/>
+          <a:ext cx="1175657" cy="411180"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -19882,13 +21090,22 @@
             </a:lnSpc>
           </a:pPr>
           <a:r>
-            <a:rPr lang="th-TH" sz="1100">
+            <a:rPr lang="th-TH" sz="1100" baseline="0">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
               <a:latin typeface="Calibri"/>
             </a:rPr>
-            <a:t>ตามที่สหกิจที่มี</a:t>
+            <a:t>ทำ </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+            </a:rPr>
+            <a:t>front-end</a:t>
           </a:r>
           <a:endParaRPr/>
         </a:p>
@@ -19912,290 +21129,27 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>23</xdr:col>
-      <xdr:colOff>297180</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>403860</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>24</xdr:col>
-      <xdr:colOff>274320</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>381000</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="322" name="สี่เหลี่ยมผืนผ้า 321"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="15544800" y="10568940"/>
-          <a:ext cx="640080" cy="419100"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:r>
-            <a:rPr lang="th-TH" sz="1000"/>
-            <a:t>ตัดเล็บ</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>23</xdr:col>
-      <xdr:colOff>411480</xdr:colOff>
-      <xdr:row>45</xdr:row>
-      <xdr:rowOff>434340</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>24</xdr:col>
-      <xdr:colOff>388620</xdr:colOff>
-      <xdr:row>46</xdr:row>
-      <xdr:rowOff>411480</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="323" name="สี่เหลี่ยมผืนผ้า 322"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="15659100" y="20322540"/>
-          <a:ext cx="640080" cy="419100"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:r>
-            <a:rPr lang="th-TH" sz="1000"/>
-            <a:t>ตัดเล็บ</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>22</xdr:col>
-      <xdr:colOff>547552</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>419100</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>24</xdr:col>
-      <xdr:colOff>478972</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>396240</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="324" name="สี่เหลี่ยมผืนผ้า 323"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="15156181" y="5774871"/>
-          <a:ext cx="1259477" cy="423455"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="tx2">
-            <a:lumMod val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:r>
-            <a:rPr lang="th-TH" sz="1000"/>
-            <a:t>สร้าง </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1000"/>
-            <a:t>Ritual </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="th-TH" sz="1000"/>
-            <a:t>สำหรับ ตอนอยู่สิงค์โปร์</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>22</xdr:col>
-      <xdr:colOff>559525</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>9797</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>24</xdr:col>
-      <xdr:colOff>490945</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>433251</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="325" name="สี่เหลี่ยมผืนผ้า 324"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="15168154" y="6258197"/>
-          <a:ext cx="1259477" cy="423454"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="tx2">
-            <a:lumMod val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:r>
-            <a:rPr lang="th-TH" sz="1000"/>
-            <a:t>สร้าง </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1000"/>
-            <a:t>Ritual </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="th-TH" sz="1000"/>
-            <a:t>สำหรับ ตอนสหกิจ</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="th-TH" sz="1000" baseline="0"/>
-            <a:t> </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1000" baseline="0"/>
-            <a:t>Part 1</a:t>
-          </a:r>
-          <a:endParaRPr lang="th-TH" sz="1000"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>544286</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>35922</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>391886</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>787</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="327" name="CustomShape 1"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="7848600" y="5391693"/>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>315684</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>14150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>163284</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>425330</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="342" name="CustomShape 1"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10276113" y="6708864"/>
           <a:ext cx="1175657" cy="411180"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -20262,119 +21216,25 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>326572</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>21771</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>326571</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>425331</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="328" name="CustomShape 1"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="8958943" y="10287000"/>
-          <a:ext cx="1328057" cy="403560"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:srgbClr val="E46C0A"/>
-        </a:solidFill>
-        <a:ln w="25560">
-          <a:solidFill>
-            <a:srgbClr val="3A5F8B"/>
-          </a:solidFill>
-          <a:round/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:txBody>
-        <a:bodyPr lIns="90000" tIns="45000" rIns="90000" bIns="45000"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:lnSpc>
-              <a:spcPct val="100000"/>
-            </a:lnSpc>
-          </a:pPr>
-          <a:r>
-            <a:rPr lang="th-TH" sz="1100" baseline="0">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-              <a:latin typeface="Calibri"/>
-            </a:rPr>
-            <a:t>ประสานงาน </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" baseline="0">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-              <a:latin typeface="Calibri"/>
-            </a:rPr>
-            <a:t>Web App </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="th-TH" sz="1100" baseline="0">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-              <a:latin typeface="Calibri"/>
-            </a:rPr>
-            <a:t>กับปราง</a:t>
-          </a:r>
-          <a:endParaRPr/>
-        </a:p>
-        <a:p>
-          <a:pPr>
-            <a:lnSpc>
-              <a:spcPct val="100000"/>
-            </a:lnSpc>
-          </a:pPr>
-          <a:endParaRPr/>
-        </a:p>
-        <a:p>
-          <a:pPr>
-            <a:lnSpc>
-              <a:spcPct val="100000"/>
-            </a:lnSpc>
-          </a:pPr>
-          <a:endParaRPr/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>179614</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>6531</xdr:rowOff>
+      <xdr:colOff>120832</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>2178</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>651574</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>409971</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="329" name="CustomShape 1"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="4827814" y="10271760"/>
+      <xdr:colOff>592792</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>405618</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="343" name="CustomShape 1"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4769032" y="6696892"/>
           <a:ext cx="471960" cy="403440"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -20416,32 +21276,215 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>56605</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>3265</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>29391</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>48986</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>6531</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>21771</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="344" name="สี่เหลี่ยมผืนผ้า 343"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5341620" y="6743700"/>
+          <a:ext cx="641168" cy="419100"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="th-TH" sz="1000"/>
+            <a:t>เดินทาง</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
       <xdr:col>20</xdr:col>
-      <xdr:colOff>33746</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>422365</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="326" name="สี่เหลี่ยมผืนผ้า 325"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="11345091" y="10268494"/>
+      <xdr:colOff>377736</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>410391</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>353787</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>383177</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="345" name="สี่เหลี่ยมผืนผ้า 344"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13658307" y="6658791"/>
+          <a:ext cx="640080" cy="419100"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="th-TH" sz="1000"/>
+            <a:t>เดินทาง</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>161108</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>18504</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>424541</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>437604</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="347" name="สี่เหลี่ยมผืนผ้า 346"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12777651" y="14300561"/>
+          <a:ext cx="3583576" cy="419100"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent4">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="th-TH" sz="1100"/>
+            <a:t>นอน</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t> / Sleep</a:t>
+          </a:r>
+          <a:endParaRPr lang="th-TH" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>187235</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>3266</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>164375</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>422366</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="348" name="สี่เหลี่ยมผืนผ้า 347"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13467806" y="12500066"/>
           <a:ext cx="1969226" cy="419100"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
         <a:solidFill>
-          <a:schemeClr val="accent2"/>
+          <a:schemeClr val="accent4">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
         </a:solidFill>
       </xdr:spPr>
       <xdr:style>
@@ -20471,7 +21514,15 @@
           </a:r>
           <a:r>
             <a:rPr lang="en-US" sz="1000"/>
-            <a:t>Hackaton Web App</a:t>
+            <a:t>Fic </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="th-TH" sz="1000"/>
+            <a:t>และ</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="th-TH" sz="1000" baseline="0"/>
+            <a:t> เพลง ลง โทรศัพท์ ไว้อ่านฟังบนเคครื่องบิน</a:t>
           </a:r>
           <a:endParaRPr lang="th-TH" sz="1000"/>
         </a:p>
@@ -20479,230 +21530,279 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>304801</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>176348</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>3266</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>87086</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>422366</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="349" name="สี่เหลี่ยมผืนผ้า 348"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="14120948" y="10714809"/>
+          <a:ext cx="1902824" cy="419100"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent4">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="th-TH" sz="1000"/>
+            <a:t>เตรียม </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1000"/>
+            <a:t>Fic </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="th-TH" sz="1000"/>
+            <a:t>และ</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="th-TH" sz="1000" baseline="0"/>
+            <a:t> เพลง ลง โทรศัพท์ ไว้อ่านฟังบนเคครื่องบิน</a:t>
+          </a:r>
+          <a:endParaRPr lang="th-TH" sz="1000"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>243840</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>18506</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>413657</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>437606</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="350" name="สี่เหลี่ยมผืนผ้า 349"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="14852469" y="11176363"/>
+          <a:ext cx="2161902" cy="419100"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent4">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="th-TH" sz="1000"/>
+            <a:t>เตรียมเสื้อผ้าที่เหมาะสมที่สุดสำหรับทริป</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="th-TH" sz="1000" baseline="0"/>
+            <a:t> เก็ยไว้สำหรับวันนั้น เผื่อเวลา</a:t>
+          </a:r>
+          <a:endParaRPr lang="th-TH" sz="1000"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>56606</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>57695</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>413657</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>30481</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="351" name="สี่เหลี่ยมผืนผ้า 350"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="16657320" y="12554495"/>
+          <a:ext cx="1021080" cy="419100"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent4">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1000"/>
+            <a:t>Charge Phone</a:t>
+          </a:r>
+          <a:endParaRPr lang="th-TH" sz="1000"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>403560</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="330" name="CustomShape 1"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="6281058" y="5355771"/>
-          <a:ext cx="1328056" cy="403560"/>
+      <xdr:colOff>644434</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>68581</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>468085</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>41367</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="352" name="สี่เหลี่ยมผืนผ้า 351"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7948748" y="14350638"/>
+          <a:ext cx="2479766" cy="419100"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
         <a:solidFill>
-          <a:srgbClr val="E46C0A"/>
+          <a:srgbClr val="002060"/>
         </a:solidFill>
-        <a:ln w="25560">
-          <a:solidFill>
-            <a:srgbClr val="3A5F8B"/>
-          </a:solidFill>
-          <a:round/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:txBody>
-        <a:bodyPr lIns="90000" tIns="45000" rIns="90000" bIns="45000"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:lnSpc>
-              <a:spcPct val="100000"/>
-            </a:lnSpc>
-          </a:pPr>
-          <a:r>
-            <a:rPr lang="th-TH" sz="1100" baseline="0">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-              <a:latin typeface="Calibri"/>
-            </a:rPr>
-            <a:t>ทำใบนัดอันใหม่ที่ คลินิกเสนานิเวช</a:t>
-          </a:r>
-          <a:endParaRPr/>
-        </a:p>
-        <a:p>
-          <a:pPr>
-            <a:lnSpc>
-              <a:spcPct val="100000"/>
-            </a:lnSpc>
-          </a:pPr>
-          <a:endParaRPr/>
-        </a:p>
-        <a:p>
-          <a:pPr>
-            <a:lnSpc>
-              <a:spcPct val="100000"/>
-            </a:lnSpc>
-          </a:pPr>
-          <a:endParaRPr/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>379912</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>54429</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>501832</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>435429</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="331" name="CustomShape 1"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="7684226" y="5410200"/>
-          <a:ext cx="1449977" cy="381000"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:srgbClr val="00B050"/>
-        </a:solidFill>
-        <a:ln w="25560">
-          <a:solidFill>
-            <a:srgbClr val="3A5F8B"/>
-          </a:solidFill>
-          <a:round/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:txBody>
-        <a:bodyPr lIns="90000" tIns="45000" rIns="90000" bIns="45000"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:lnSpc>
-              <a:spcPct val="100000"/>
-            </a:lnSpc>
-          </a:pPr>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-              <a:latin typeface="Calibri"/>
-            </a:rPr>
-            <a:t>relax</a:t>
-          </a:r>
-          <a:endParaRPr/>
-        </a:p>
-        <a:p>
-          <a:pPr>
-            <a:lnSpc>
-              <a:spcPct val="100000"/>
-            </a:lnSpc>
-          </a:pPr>
-          <a:endParaRPr/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>119742</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>438693</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>22</xdr:col>
-      <xdr:colOff>631370</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>403558</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="332" name="CustomShape 1"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="14064342" y="5794464"/>
-          <a:ext cx="1175657" cy="411180"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:srgbClr val="E46C0A"/>
-        </a:solidFill>
-        <a:ln w="25560">
-          <a:solidFill>
-            <a:srgbClr val="3A5F8B"/>
-          </a:solidFill>
-          <a:round/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:txBody>
-        <a:bodyPr lIns="90000" tIns="45000" rIns="90000" bIns="45000"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:lnSpc>
-              <a:spcPct val="100000"/>
-            </a:lnSpc>
-          </a:pPr>
-          <a:r>
-            <a:rPr lang="th-TH" sz="1100" baseline="0">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-              <a:latin typeface="Calibri"/>
-            </a:rPr>
-            <a:t>ทำ </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" baseline="0">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-              <a:latin typeface="Calibri"/>
-            </a:rPr>
-            <a:t>front-end</a:t>
-          </a:r>
-          <a:endParaRPr/>
-        </a:p>
-        <a:p>
-          <a:pPr>
-            <a:lnSpc>
-              <a:spcPct val="100000"/>
-            </a:lnSpc>
-          </a:pPr>
-          <a:endParaRPr/>
-        </a:p>
-        <a:p>
-          <a:pPr>
-            <a:lnSpc>
-              <a:spcPct val="100000"/>
-            </a:lnSpc>
-          </a:pPr>
-          <a:endParaRPr/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="th-TH" sz="1000"/>
+            <a:t>เตรียมของ ใช้ </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1000"/>
+            <a:t>Ritual </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="th-TH" sz="1000"/>
+            <a:t>พิเศษ สำหรับ </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1000"/>
+            <a:t>Trip</a:t>
+          </a:r>
+          <a:endParaRPr lang="th-TH" sz="1000"/>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -58097,8 +59197,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="W15" sqref="W15"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="AA31" sqref="AA31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>